<commit_message>
[IMP] Transdoo upgrade (PO state) & test
</commit_message>
<xml_diff>
--- a/odoo_default_tnl.xlsx
+++ b/odoo_default_tnl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="2974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="2976">
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -8234,6 +8234,12 @@
   </si>
   <si>
     <t xml:space="preserve">Totale IVA a debito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totale dovuto</t>
   </si>
   <si>
     <t xml:space="preserve">Total in Company Currency</t>
@@ -9042,13 +9048,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1579"/>
+  <dimension ref="A1:C1580"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A995" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1008" activeCellId="0" sqref="C1008"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1574" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1580" activeCellId="0" sqref="A1:C1580"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.39"/>
@@ -20731,15 +20737,15 @@
         <v>2758</v>
       </c>
       <c r="C1458" s="0" t="s">
-        <v>956</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="1459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1459" s="0" t="s">
-        <v>2759</v>
+        <v>2760</v>
       </c>
       <c r="C1459" s="0" t="s">
-        <v>2760</v>
+        <v>956</v>
       </c>
     </row>
     <row r="1460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20747,15 +20753,15 @@
         <v>2761</v>
       </c>
       <c r="C1460" s="0" t="s">
-        <v>1582</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="1461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1461" s="0" t="s">
-        <v>2762</v>
+        <v>2763</v>
       </c>
       <c r="C1461" s="0" t="s">
-        <v>2763</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="1462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20779,23 +20785,23 @@
         <v>2768</v>
       </c>
       <c r="C1464" s="0" t="s">
-        <v>2719</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="1465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1465" s="0" t="s">
-        <v>2769</v>
+        <v>2770</v>
       </c>
       <c r="C1465" s="0" t="s">
-        <v>1235</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="1466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1466" s="0" t="s">
-        <v>2770</v>
+        <v>2771</v>
       </c>
       <c r="C1466" s="0" t="s">
-        <v>2771</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20835,15 +20841,15 @@
         <v>2780</v>
       </c>
       <c r="C1471" s="0" t="s">
-        <v>805</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="1472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1472" s="0" t="s">
-        <v>2781</v>
+        <v>2782</v>
       </c>
       <c r="C1472" s="0" t="s">
-        <v>2782</v>
+        <v>805</v>
       </c>
     </row>
     <row r="1473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20872,15 +20878,15 @@
     </row>
     <row r="1476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1476" s="0" t="s">
-        <v>2787</v>
+        <v>2789</v>
       </c>
       <c r="C1476" s="0" t="s">
-        <v>2789</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="1477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1477" s="0" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="C1477" s="0" t="s">
         <v>2791</v>
@@ -20907,15 +20913,15 @@
         <v>2796</v>
       </c>
       <c r="C1480" s="0" t="s">
-        <v>231</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="1481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1481" s="0" t="s">
-        <v>2797</v>
+        <v>2798</v>
       </c>
       <c r="C1481" s="0" t="s">
-        <v>2798</v>
+        <v>231</v>
       </c>
     </row>
     <row r="1482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20952,10 +20958,10 @@
     </row>
     <row r="1486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1486" s="0" t="s">
-        <v>2805</v>
+        <v>2807</v>
       </c>
       <c r="C1486" s="0" t="s">
-        <v>2806</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="1487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21035,23 +21041,23 @@
         <v>2825</v>
       </c>
       <c r="C1496" s="0" t="s">
-        <v>2584</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="1497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1497" s="0" t="s">
-        <v>2826</v>
+        <v>2827</v>
       </c>
       <c r="C1497" s="0" t="s">
-        <v>2626</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="1498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1498" s="0" t="s">
-        <v>2827</v>
+        <v>2828</v>
       </c>
       <c r="C1498" s="0" t="s">
-        <v>2828</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="1499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21107,12 +21113,12 @@
         <v>2841</v>
       </c>
       <c r="C1505" s="0" t="s">
-        <v>207</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="1506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1506" s="0" t="s">
-        <v>2842</v>
+        <v>2843</v>
       </c>
       <c r="C1506" s="0" t="s">
         <v>207</v>
@@ -21120,34 +21126,34 @@
     </row>
     <row r="1507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1507" s="0" t="s">
-        <v>2843</v>
+        <v>2844</v>
       </c>
       <c r="C1507" s="0" t="s">
-        <v>2840</v>
+        <v>207</v>
       </c>
     </row>
     <row r="1508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1508" s="0" t="s">
-        <v>2844</v>
+        <v>2845</v>
       </c>
       <c r="C1508" s="0" t="s">
-        <v>2840</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="1509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1509" s="0" t="s">
-        <v>2845</v>
+        <v>2846</v>
       </c>
       <c r="C1509" s="0" t="s">
-        <v>2840</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="1510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1510" s="0" t="s">
-        <v>2846</v>
+        <v>2847</v>
       </c>
       <c r="C1510" s="0" t="s">
-        <v>2847</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="1511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21168,15 +21174,15 @@
     </row>
     <row r="1513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1513" s="0" t="s">
-        <v>2850</v>
+        <v>2852</v>
       </c>
       <c r="C1513" s="0" t="s">
-        <v>2852</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="1514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1514" s="0" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="C1514" s="0" t="s">
         <v>2854</v>
@@ -21200,15 +21206,15 @@
     </row>
     <row r="1517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1517" s="0" t="s">
-        <v>2857</v>
+        <v>2859</v>
       </c>
       <c r="C1517" s="0" t="s">
-        <v>2859</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="1518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1518" s="0" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="C1518" s="0" t="s">
         <v>2861</v>
@@ -21264,10 +21270,10 @@
     </row>
     <row r="1525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1525" s="0" t="s">
-        <v>2872</v>
+        <v>2874</v>
       </c>
       <c r="C1525" s="0" t="s">
-        <v>2873</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="1526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21283,15 +21289,15 @@
         <v>2876</v>
       </c>
       <c r="C1527" s="0" t="s">
-        <v>207</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="1528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1528" s="0" t="s">
-        <v>2877</v>
+        <v>2878</v>
       </c>
       <c r="C1528" s="0" t="s">
-        <v>2878</v>
+        <v>207</v>
       </c>
     </row>
     <row r="1529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21299,15 +21305,15 @@
         <v>2879</v>
       </c>
       <c r="C1529" s="0" t="s">
-        <v>2545</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="1530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1530" s="0" t="s">
-        <v>2880</v>
+        <v>2881</v>
       </c>
       <c r="C1530" s="0" t="s">
-        <v>2881</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="1531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21355,12 +21361,12 @@
         <v>2892</v>
       </c>
       <c r="C1536" s="0" t="s">
-        <v>2892</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="1537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1537" s="0" t="s">
-        <v>2893</v>
+        <v>2894</v>
       </c>
       <c r="C1537" s="0" t="s">
         <v>2894</v>
@@ -21371,23 +21377,23 @@
         <v>2895</v>
       </c>
       <c r="C1538" s="0" t="s">
-        <v>2894</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="1539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1539" s="0" t="s">
+        <v>2897</v>
+      </c>
+      <c r="C1539" s="0" t="s">
         <v>2896</v>
-      </c>
-      <c r="C1539" s="0" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="1540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1540" s="0" t="s">
-        <v>2897</v>
+        <v>2898</v>
       </c>
       <c r="C1540" s="0" t="s">
-        <v>2898</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21427,15 +21433,15 @@
         <v>2907</v>
       </c>
       <c r="C1545" s="0" t="s">
-        <v>771</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="1546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1546" s="0" t="s">
-        <v>2908</v>
+        <v>2909</v>
       </c>
       <c r="C1546" s="0" t="s">
-        <v>2909</v>
+        <v>771</v>
       </c>
     </row>
     <row r="1547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21587,15 +21593,15 @@
         <v>2946</v>
       </c>
       <c r="C1565" s="0" t="s">
-        <v>1001</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="1566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1566" s="0" t="s">
-        <v>2947</v>
+        <v>2948</v>
       </c>
       <c r="C1566" s="0" t="s">
-        <v>2948</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21619,15 +21625,15 @@
         <v>2953</v>
       </c>
       <c r="C1569" s="0" t="s">
-        <v>14</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="1570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1570" s="0" t="s">
-        <v>2954</v>
+        <v>2955</v>
       </c>
       <c r="C1570" s="0" t="s">
-        <v>2955</v>
+        <v>14</v>
       </c>
     </row>
     <row r="1571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21700,6 +21706,14 @@
       </c>
       <c r="C1579" s="0" t="s">
         <v>2973</v>
+      </c>
+    </row>
+    <row r="1580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1580" s="0" t="s">
+        <v>2974</v>
+      </c>
+      <c r="C1580" s="0" t="s">
+        <v>2975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] zerobug + z0lib_odoo + travis_emulator + z0lib: upgrades
</commit_message>
<xml_diff>
--- a/odoo_default_tnl.xlsx
+++ b/odoo_default_tnl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9075" uniqueCount="8589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9079" uniqueCount="8592">
   <si>
     <t xml:space="preserve">module</t>
   </si>
@@ -10304,10 +10304,10 @@
     <t xml:space="preserve">Trovati record multipli in base al campo '%%(field)s' (%d trovati)</t>
   </si>
   <si>
-    <t xml:space="preserve">Found multiple records.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rilevati più record.</t>
+    <t xml:space="preserve">Found multiple records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rilevati più record</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
@@ -27392,6 +27392,15 @@
   </si>
   <si>
     <t xml:space="preserve">CAP non impostato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry-run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File dati Excel</t>
   </si>
 </sst>
 </file>
@@ -27505,13 +27514,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4593"/>
+  <dimension ref="A1:C4595"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3020" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3035" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1783" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1796" activeCellId="0" sqref="C1796"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.12"/>
@@ -63931,6 +63940,22 @@
       </c>
       <c r="C4593" s="0" t="s">
         <v>8588</v>
+      </c>
+    </row>
+    <row r="4594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4594" s="0" t="s">
+        <v>8589</v>
+      </c>
+      <c r="C4594" s="0" t="s">
+        <v>8590</v>
+      </c>
+    </row>
+    <row r="4595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4595" s="0" t="s">
+        <v>3016</v>
+      </c>
+      <c r="C4595" s="0" t="s">
+        <v>8591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>